<commit_message>
validate excel input (50%)
</commit_message>
<xml_diff>
--- a/DormManagement/Server/download/template.xlsx
+++ b/DormManagement/Server/download/template.xlsx
@@ -5,15 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ForStudy_2017\互联网技术\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\TinyHeart\DormManagement\Server\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14238" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14238" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,59 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>楼号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宿舍号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>床位编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态（空床／已入住）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已入住学号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已入住学生姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>格式：数字
-eg: 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>格式：数字
-空床：0
-已入住：1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>格式：数字
-男：0
-女：1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5214（5号楼-2楼14号屋）
-E1224（13号楼-1单元-2层-2号门-4号屋）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -116,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,23 +76,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="DengXian"/>
       <family val="2"/>
       <charset val="134"/>
@@ -187,19 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -480,78 +405,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.37890625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="2"/>
-    <col min="3" max="3" width="18.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" style="2"/>
-    <col min="6" max="6" width="20.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="2"/>
-    <col min="8" max="8" width="16.47265625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="75">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -560,41 +413,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.90234375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.94921875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.94921875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.37890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.09375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.76171875" style="5"/>
+    <col min="1" max="1" width="6.90234375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="47.94921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.94921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.37890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.09375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.76171875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>18</v>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>